<commit_message>
multi OS Test Options and Test Properties
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/98cbadd423e0d27c/Documents/Studies_and_Certs/Automation_Testing_Masters/Phase_2/Final_Project_WS/Eclipse_2018-09_Mac/swiggy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/98cbadd423e0d27c/Documents/Studies_and_Certs/Automation_Testing_Masters/Phase_2/Final_Project_WS/Eclipse_2018-08_Win/swiggy/SimplilearnSwiggy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68100925-6B4E-9145-9C48-9D101A4A82C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{68100925-6B4E-9145-9C48-9D101A4A82C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A008839A-7A51-4763-8B66-9433410F7ABF}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14200" xr2:uid="{CB877AC6-41DC-094B-94B6-13DB16BB9D23}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="15375" windowHeight="7875" xr2:uid="{CB877AC6-41DC-094B-94B6-13DB16BB9D23}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="SignUp" sheetId="2" r:id="rId2"/>
+    <sheet name="FoodSearch" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>loginid</t>
   </si>
@@ -63,7 +65,16 @@
     <t>8097253791</t>
   </si>
   <si>
-    <t>safari</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Thane</t>
+  </si>
+  <si>
+    <t>Vashi</t>
   </si>
 </sst>
 </file>
@@ -419,12 +430,12 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,7 +446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -446,7 +457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -457,15 +468,91 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{975A0691-4CBF-4F1B-8EBC-DED138803075}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E44974-E572-4383-BF0D-B29273646932}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>